<commit_message>
Subindo esboço da aula 04
</commit_message>
<xml_diff>
--- a/aula03/estudo-tempo.xlsx
+++ b/aula03/estudo-tempo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27518"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leandro.salenave\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\181810032\Desktop\Mineracao_Analise_Dados\aula03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{5E49CE77-BFE1-44DC-8567-F617CDC654D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D08BA68-DDF7-4B4E-AB7F-BA1BAEB9D42B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55299963-1186-49B1-8021-51F4886E8C42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C164498E-2B99-413C-BB3F-B932DC0A3EF3}"/>
   </bookViews>
@@ -20,17 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -90,8 +79,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -119,9 +116,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,16 +454,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF561B62-40C4-41F3-864A-9DD1FBC56133}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -561,6 +559,9 @@
       <c r="C10" s="1">
         <v>45370</v>
       </c>
+      <c r="D10" s="1">
+        <v>45381</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
@@ -569,6 +570,12 @@
       <c r="B11" t="s">
         <v>12</v>
       </c>
+      <c r="C11" s="1">
+        <v>45381</v>
+      </c>
+      <c r="D11" s="1">
+        <v>45381</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
@@ -577,6 +584,12 @@
       <c r="B12" t="s">
         <v>13</v>
       </c>
+      <c r="C12" s="1">
+        <v>45381</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45381</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
@@ -585,6 +598,12 @@
       <c r="B13" t="s">
         <v>14</v>
       </c>
+      <c r="C13" s="1">
+        <v>45381</v>
+      </c>
+      <c r="D13" s="1">
+        <v>45381</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
@@ -593,8 +612,26 @@
       <c r="B14" t="s">
         <v>15</v>
       </c>
+      <c r="C14" s="1">
+        <v>45381</v>
+      </c>
+      <c r="D14" s="1">
+        <v>45381</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="C15" s="1">
+        <v>45384</v>
+      </c>
+      <c r="D15" s="1">
+        <v>45384</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="D20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>